<commit_message>
Prod - Support Update
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/Prod/ALL_PAGES/END_TO_END/TC15_Verify_UserRegistration.xlsx
+++ b/Input_files/Actual_testcases/Kaman/Prod/ALL_PAGES/END_TO_END/TC15_Verify_UserRegistration.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23231"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMANLiveBranch\Input_files\Actual_testcases\Kaman\Prod\ALL_PAGES\END_TO_END\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Vaibhav Oza\KAMAN_ECTEST_IE_SANITY-master\Input_files\Actual_testcases\Kaman\Prod\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F70EBE37-BC97-4D1C-8306-1B2D1A69300F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="TC15_Verify_UserRegistration" sheetId="1" r:id="rId1"/>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="52">
   <si>
     <t>TestCase</t>
   </si>
@@ -182,7 +181,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -603,11 +602,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G19" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -659,38 +658,34 @@
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E4" s="3"/>
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2"/>
-      <c r="B5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>12</v>
+      <c r="B5" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2"/>
       <c r="B6" s="3" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>26</v>
@@ -699,8 +694,8 @@
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2"/>
-      <c r="B7" s="2" t="s">
-        <v>11</v>
+      <c r="B7" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>13</v>
@@ -708,27 +703,27 @@
       <c r="D7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>13</v>
-      </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2"/>
-      <c r="B8" s="3" t="s">
-        <v>28</v>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2"/>
-      <c r="B9" s="2" t="s">
-        <v>11</v>
+      <c r="B9" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>14</v>
@@ -736,27 +731,27 @@
       <c r="D9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>14</v>
-      </c>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2"/>
-      <c r="B10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>15</v>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="3" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2"/>
-      <c r="B11" s="2" t="s">
-        <v>20</v>
+      <c r="B11" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>15</v>
@@ -764,27 +759,27 @@
       <c r="D11" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="E11" s="3"/>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2"/>
-      <c r="B12" s="3" t="s">
-        <v>28</v>
+      <c r="B12" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2"/>
-      <c r="B13" s="2" t="s">
-        <v>11</v>
+      <c r="B13" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>16</v>
@@ -792,36 +787,36 @@
       <c r="D13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>16</v>
-      </c>
+      <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2"/>
-      <c r="B14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="B14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2"/>
       <c r="B15" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>26</v>
-      </c>
+        <v>48</v>
+      </c>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2"/>
-      <c r="B16" s="2" t="s">
-        <v>11</v>
+      <c r="B16" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>17</v>
@@ -829,27 +824,27 @@
       <c r="D16" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>17</v>
-      </c>
+      <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2"/>
-      <c r="B17" s="3" t="s">
-        <v>28</v>
+      <c r="B17" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2"/>
-      <c r="B18" s="2" t="s">
-        <v>11</v>
+      <c r="B18" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>18</v>
@@ -857,105 +852,109 @@
       <c r="D18" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2"/>
-      <c r="B19" s="3" t="s">
-        <v>35</v>
+      <c r="B19" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2"/>
       <c r="B20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2"/>
       <c r="B21" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>39</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2"/>
       <c r="B22" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2"/>
       <c r="B23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>40</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2"/>
       <c r="B24" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2"/>
       <c r="B25" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D25" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>42</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2"/>
       <c r="B26" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2"/>
@@ -978,30 +977,26 @@
     <row r="29" spans="1:5">
       <c r="A29" s="2"/>
       <c r="B29" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>19</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2"/>
       <c r="B30" s="3" t="s">
-        <v>9</v>
+        <v>31</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2"/>
@@ -1009,12 +1004,25 @@
         <v>9</v>
       </c>
       <c r="C31" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="2"/>
+      <c r="B32" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E31" s="2"/>
+      <c r="D32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
@@ -1024,11 +1032,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1159,9 +1167,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" xr:uid="{543BF58E-8AD1-4B7D-BD30-1A8F4861C8AD}"/>
-    <hyperlink ref="B6" r:id="rId2" xr:uid="{3FFE1B31-A72E-4053-A2A7-9A716823392A}"/>
-    <hyperlink ref="B7" r:id="rId3" xr:uid="{C0969BF1-9A25-441E-8565-A496082B4317}"/>
+    <hyperlink ref="B5" r:id="rId1"/>
+    <hyperlink ref="B6" r:id="rId2"/>
+    <hyperlink ref="B7" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1177,6 +1185,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006B9247FD3B8DCE459B42E632A3609B44" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="3308c0b5f2a874e4881ed9e3e8048963">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1a153bf7-9590-4a62-91b6-0515f1c483dc" xmlns:ns3="fd27ab66-8f5a-4733-8e24-c3cb82244a05" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="afaafca1b8c32e4865f6f60996200392" ns2:_="" ns3:_="">
     <xsd:import namespace="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
@@ -1373,12 +1387,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75986BA1-ED37-4C63-93A8-4C325EA50F3E}">
   <ds:schemaRefs>
@@ -1388,6 +1396,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="fd27ab66-8f5a-4733-8e24-c3cb82244a05"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73F47607-34AD-43FE-B910-18186D4DE9CC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1404,21 +1429,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{201F13FF-ABE4-451A-88FD-FA1FE3D91855}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1a153bf7-9590-4a62-91b6-0515f1c483dc"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="fd27ab66-8f5a-4733-8e24-c3cb82244a05"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>